<commit_message>
A bit more complex still
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A57266C-867D-3B43-B2EE-97A81DA8E494}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09CDCB70-51DD-E74D-B1E5-3869EC5B2931}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Alpha, Jan</t>
-  </si>
-  <si>
     <t>&lt;placeholder&gt;</t>
   </si>
   <si>
@@ -119,13 +116,22 @@
     <t>Source row value</t>
   </si>
   <si>
-    <t>Target intersection of Jan and Alpha</t>
-  </si>
-  <si>
     <t>Summary!C5</t>
   </si>
   <si>
     <t>Put in C5</t>
+  </si>
+  <si>
+    <t>matches</t>
+  </si>
+  <si>
+    <t>Mar.*</t>
+  </si>
+  <si>
+    <t>Target intersection of Mar (using a regex search in caes it says March) and Beta</t>
+  </si>
+  <si>
+    <t>Table search</t>
   </si>
 </sst>
 </file>
@@ -521,13 +527,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
   <dimension ref="B3:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.22265625" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5078125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -535,15 +542,15 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -558,20 +565,20 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
@@ -579,13 +586,13 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
@@ -595,7 +602,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -610,24 +617,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
   <dimension ref="B2:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.51171875" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.203125" customWidth="1"/>
+    <col min="2" max="2" width="17.890625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -638,43 +645,43 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -685,43 +692,43 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>-1</v>
@@ -729,41 +736,41 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Now do the loss column
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="139" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A98FA77F-2F9D-7A4A-A72D-858FEE0C3961}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAAEDABC-0447-164D-A2A1-8DCB36C385A8}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -152,12 +152,6 @@
     <t>Populate the profit row from the profit £ column</t>
   </si>
   <si>
-    <t>Match a regular expression ending in "3"</t>
-  </si>
-  <si>
-    <t>(.*) 3$</t>
-  </si>
-  <si>
     <t>Source row column offset</t>
   </si>
   <si>
@@ -174,6 +168,12 @@
   </si>
   <si>
     <t>Target row value</t>
+  </si>
+  <si>
+    <t>Loss row</t>
+  </si>
+  <si>
+    <t>Do the same for the loss row, but keep it simple this time</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
   <dimension ref="B3:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -657,10 +657,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A12" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -843,83 +843,149 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21" t="s">
-        <v>5</v>
+      <c r="D21">
+        <v>-1</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22">
-        <v>-1</v>
+      <c r="D22" t="s">
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
         <v>33</v>
       </c>
-      <c r="F23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>42</v>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test for expanding tables
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAAEDABC-0447-164D-A2A1-8DCB36C385A8}"/>
+  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDCF0A73-FA7F-CD47-A7D1-1366D4EBAABB}"/>
   <bookViews>
     <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -77,18 +77,12 @@
     <t>Import date</t>
   </si>
   <si>
-    <t>Cell</t>
-  </si>
-  <si>
     <t>Sheet</t>
   </si>
   <si>
     <t>Report 1</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>Target cell</t>
   </si>
   <si>
@@ -174,6 +168,39 @@
   </si>
   <si>
     <t>Do the same for the loss row, but keep it simple this time</t>
+  </si>
+  <si>
+    <t>Copy and expand a table</t>
+  </si>
+  <si>
+    <t>Copy a single value from a table using a search on row/column labels</t>
+  </si>
+  <si>
+    <t>Copy a single value by searching for its label</t>
+  </si>
+  <si>
+    <t>Cell value</t>
+  </si>
+  <si>
+    <t>Column offset</t>
+  </si>
+  <si>
+    <t>The label</t>
+  </si>
+  <si>
+    <t>Value is in the adjacent cell</t>
+  </si>
+  <si>
+    <t>Report 2</t>
+  </si>
+  <si>
+    <t>RangleTable</t>
+  </si>
+  <si>
+    <t>PlanTable</t>
+  </si>
+  <si>
+    <t>Expand</t>
   </si>
 </sst>
 </file>
@@ -570,7 +597,7 @@
   <dimension ref="B3:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -589,7 +616,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>4</v>
@@ -657,10 +684,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
-  <dimension ref="B2:F31"/>
+  <dimension ref="B2:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -693,299 +720,380 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
-        <v>18</v>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
+      <c r="B9" s="1"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12">
-        <v>-1</v>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
+      <c r="F18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="s">
-        <v>33</v>
+      <c r="D19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="D21">
-        <v>-1</v>
+      <c r="D21" t="s">
+        <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" t="s">
-        <v>33</v>
+      <c r="D22">
+        <v>-1</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
         <v>5</v>
       </c>
-      <c r="F23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" t="s">
-        <v>45</v>
+      <c r="F24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>11</v>
       </c>
-      <c r="D27" t="s">
-        <v>33</v>
+      <c r="D27" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
-      <c r="D29">
-        <v>-1</v>
+      <c r="D29" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
       </c>
-      <c r="D30" t="s">
-        <v>33</v>
+      <c r="D30">
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct test data error
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDCF0A73-FA7F-CD47-A7D1-1366D4EBAABB}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BCE40C-CD04-6947-BD40-E2B9C3CBE672}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -170,18 +170,12 @@
     <t>Do the same for the loss row, but keep it simple this time</t>
   </si>
   <si>
-    <t>Copy and expand a table</t>
-  </si>
-  <si>
     <t>Copy a single value from a table using a search on row/column labels</t>
   </si>
   <si>
     <t>Copy a single value by searching for its label</t>
   </si>
   <si>
-    <t>Cell value</t>
-  </si>
-  <si>
     <t>Column offset</t>
   </si>
   <si>
@@ -191,16 +185,7 @@
     <t>Value is in the adjacent cell</t>
   </si>
   <si>
-    <t>Report 2</t>
-  </si>
-  <si>
-    <t>RangleTable</t>
-  </si>
-  <si>
-    <t>PlanTable</t>
-  </si>
-  <si>
-    <t>Expand</t>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -596,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
   <dimension ref="B3:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -684,10 +669,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
-  <dimension ref="B2:F38"/>
+  <dimension ref="B2:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -721,7 +706,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
@@ -737,7 +722,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -746,12 +731,12 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -760,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
@@ -788,7 +773,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
@@ -1036,64 +1021,6 @@
       </c>
       <c r="D32" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempt to do table expansion again
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7BCE40C-CD04-6947-BD40-E2B9C3CBE672}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9386B77-41F9-D941-A25F-0478353949F9}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -185,7 +185,25 @@
     <t>Value is in the adjacent cell</t>
   </si>
   <si>
+    <t>RangleTable</t>
+  </si>
+  <si>
+    <t>PlanTable</t>
+  </si>
+  <si>
+    <t>Expand</t>
+  </si>
+  <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Replace table</t>
+  </si>
+  <si>
+    <t>(Yes, it’s a typo)</t>
+  </si>
+  <si>
+    <t>Copy from one table to another</t>
   </si>
 </sst>
 </file>
@@ -581,9 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
   <dimension ref="B3:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -669,10 +685,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
-  <dimension ref="B2:F32"/>
+  <dimension ref="B2:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -722,7 +738,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1021,6 +1037,56 @@
       </c>
       <c r="D32" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New table for copying range
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9386B77-41F9-D941-A25F-0478353949F9}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B072C25-A406-4D45-B927-64C37F6709D5}"/>
   <bookViews>
     <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -188,9 +188,6 @@
     <t>RangleTable</t>
   </si>
   <si>
-    <t>PlanTable</t>
-  </si>
-  <si>
     <t>Expand</t>
   </si>
   <si>
@@ -204,6 +201,15 @@
   </si>
   <si>
     <t>Copy from one table to another</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Table3</t>
   </si>
 </sst>
 </file>
@@ -256,7 +262,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -292,11 +316,24 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{58AB90E0-8AD9-334B-9C1C-ACBD711C0293}" name="PlanTable" displayName="PlanTable" ref="B11:D13" totalsRowShown="0">
   <autoFilter ref="B11:D13" xr:uid="{7183650E-900B-D140-A269-4D6F896DB0BF}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{5C016BAD-9FBD-CE49-94E9-88445A35562D}" name="Area" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5C016BAD-9FBD-CE49-94E9-88445A35562D}" name="Area" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{34AE911A-0D98-534A-AFF6-D1C32150F548}" name="Profit"/>
     <tableColumn id="3" xr3:uid="{F7752A5B-BB37-0340-93D8-F844021C3290}" name="Loss"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{59CF296E-9158-0A4D-9B5E-16AA8BA59589}" name="Table3" displayName="Table3" ref="B15:E16" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B15:E16" xr:uid="{EDF16454-6008-114C-B871-7C3960F8F0BE}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{7D7D98A6-2BDB-8C46-9C10-0BEBBDD96AF7}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{B9F42C18-7B81-A648-818F-A8BDBA46B6D6}" name="Date"/>
+    <tableColumn id="3" xr3:uid="{DCFF12C8-0522-6C4A-A9FA-7D9EEB7F00FA}" name="Range"/>
+    <tableColumn id="4" xr3:uid="{6378C6C7-568D-CF4D-ACC3-9337B386C06F}" name="Price"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -597,9 +634,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
-  <dimension ref="B3:F13"/>
+  <dimension ref="B3:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -675,10 +714,25 @@
         <v>8</v>
       </c>
     </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -687,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
   <dimension ref="B2:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -738,7 +792,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1047,10 +1101,10 @@
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
@@ -1064,7 +1118,7 @@
         <v>49</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
@@ -1075,12 +1129,12 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Try again to get test data right :(
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D80338F-5D7D-6944-833F-50823B01D17C}"/>
+  <xr:revisionPtr revIDLastSave="237" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08A3FA28-02EA-0D45-9671-C48286F7B1C9}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -226,9 +226,6 @@
   </si>
   <si>
     <t>Expand table</t>
-  </si>
-  <si>
-    <t>Tablle</t>
   </si>
   <si>
     <t>CARS_RANGE</t>
@@ -670,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
   <dimension ref="B3:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -776,7 +773,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -789,7 +786,7 @@
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -802,7 +799,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -814,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C626B707-217E-9C4B-A063-5643146AE8A2}">
   <dimension ref="B2:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1227,18 +1224,18 @@
         <v>62</v>
       </c>
       <c r="F39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
         <v>63</v>
-      </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
@@ -1249,7 +1246,7 @@
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add more formulae and more useful chart elements
</commit_message>
<xml_diff>
--- a/src/xlsx_extract/test_data/target.xlsx
+++ b/src/xlsx_extract/test_data/target.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maraspeli/Build/Python/xlsx-extract/src/xlsx_extract/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="274" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA5C192D-2D13-EA4D-8DD3-8EB97D43AC23}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="13_ncr:1_{3AB30441-7E70-BB4B-92EF-384BB0155177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{209173EF-7E52-8F4B-9F36-C6F2D741C3CD}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6300" yWindow="2260" windowWidth="20360" windowHeight="14560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="76">
   <si>
     <t>Date</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Summary!F3</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -380,32 +383,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>P/L</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -446,11 +423,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Summary!$C$11</c:f>
+              <c:f>Summary!$D$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Profit</c:v>
+                  <c:v>Range</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -467,89 +444,19 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Summary!$B$12:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Alpha</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Beta</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Summary!$C$12:$C$13</c:f>
+              <c:f>Summary!$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-21CC-A34D-9D78-DCED788543EF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Summary!$D$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Loss</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Summary!$B$12:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Alpha</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Beta</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Summary!$D$12:$D$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-21CC-A34D-9D78-DCED788543EF}"/>
+              <c16:uniqueId val="{00000001-2E70-F749-88F7-A0596C34066F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -562,17 +469,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241883328"/>
-        <c:axId val="241888240"/>
+        <c:axId val="415759728"/>
+        <c:axId val="415830208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241883328"/>
+        <c:axId val="415759728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -609,7 +515,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241888240"/>
+        <c:crossAx val="415830208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -617,7 +523,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241888240"/>
+        <c:axId val="415830208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -668,7 +574,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241883328"/>
+        <c:crossAx val="415759728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2179,22 +2085,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>273050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>27515</xdr:rowOff>
+      <xdr:colOff>103716</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>431801</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>55032</xdr:rowOff>
+      <xdr:colOff>194734</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C0C99AE-2154-7B40-A578-A267B57807AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6B1870F-945B-AF49-A0AD-F9609B8F5C4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2580,8 +2486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD952CAC-5724-BE41-916A-7E83B1848A30}">
   <dimension ref="B3:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3255,11 +3161,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE512EF-705D-CA47-AE86-A07C92EA8213}">
-  <dimension ref="B4:C6"/>
+  <dimension ref="B4:C9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3287,6 +3191,15 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C4:C6)</f>
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>